<commit_message>
feat: Change email info on email_list.xlsx and completed mail sending
</commit_message>
<xml_diff>
--- a/week3/email_list.xlsx
+++ b/week3/email_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhn2-003/Documents/dev/KDT_HW/week3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7C43747-E1DF-2E41-92BC-5B29BA0F4FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60D76D-A3E8-AA4C-8DA0-4EE8213E7D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32860" yWindow="-260" windowWidth="26820" windowHeight="16040" xr2:uid="{285689C1-7D9B-D94E-ACE6-9F4AF12DF945}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>배프</t>
   </si>
   <si>
+    <t>송종근</t>
+  </si>
+  <si>
     <t>beap.jg@gmail.com</t>
-  </si>
-  <si>
-    <t>송종근</t>
   </si>
   <si>
     <t>masterofflash@nate.com</t>
@@ -68,20 +68,18 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
+      <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,11 +99,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -113,15 +108,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -433,13 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012201AD-D2D6-F044-AD08-BE6CCE53305D}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <cols>
+    <col min="3" max="3" width="42.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -453,33 +454,39 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="mailto:beap.jg@gmail.com" xr:uid="{8A2505AD-4545-3F41-B333-43802F268477}"/>
-    <hyperlink ref="C3" r:id="rId2" display="mailto:masterofflash@nate.com" xr:uid="{B86D9599-A434-7B4B-B125-47EBF5452F23}"/>
-  </hyperlinks>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>